<commit_message>
Updating the HTML v2
</commit_message>
<xml_diff>
--- a/data/instances.xlsx
+++ b/data/instances.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gxologistics-my.sharepoint.com/personal/xavier_parro_gxo_com/Documents/1. GXO/3. Internal/3. Developments/2. BY Instances/gxo-instances-managaer/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gxologistics-my.sharepoint.com/personal/xavier_parro_gxo_com/Documents/1. GXO/3. Internal/3. Developments/2. BY Instances Manager/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A3C676D-04FE-46A3-BA85-E52D00AEE8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{3A3C676D-04FE-46A3-BA85-E52D00AEE8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13A16423-F262-4F25-9FDB-1632211FCF09}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{3AFE9030-45BA-40A4-AA93-EF8467272483}"/>
+    <workbookView xWindow="-23148" yWindow="816" windowWidth="23256" windowHeight="13896" xr2:uid="{3AFE9030-45BA-40A4-AA93-EF8467272483}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="203">
   <si>
     <t>GXO  Account</t>
   </si>
@@ -568,12 +568,6 @@
     <t>BOLT</t>
   </si>
   <si>
-    <t>KHUMO Tyres</t>
-  </si>
-  <si>
-    <t>KHUMO</t>
-  </si>
-  <si>
     <t>https://bh10-gxo-wms-web-np4.jdadelivers.com/</t>
   </si>
   <si>
@@ -635,6 +629,24 @@
   </si>
   <si>
     <t>GE1</t>
+  </si>
+  <si>
+    <t>Kumho</t>
+  </si>
+  <si>
+    <t>Kumo Tires</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
   </si>
 </sst>
 </file>
@@ -1188,14 +1200,14 @@
   <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7265625" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.36328125" customWidth="1"/>
     <col min="4" max="4" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.6328125" bestFit="1" customWidth="1"/>
@@ -1212,13 +1224,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>2</v>
@@ -1230,25 +1242,25 @@
         <v>4</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>5</v>
@@ -1279,7 +1291,9 @@
       <c r="B2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
@@ -1333,7 +1347,9 @@
       <c r="B3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
@@ -1387,7 +1403,9 @@
       <c r="B4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10" t="s">
@@ -1441,7 +1459,9 @@
       <c r="B5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
@@ -1495,7 +1515,9 @@
       <c r="B6" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
@@ -1549,7 +1571,9 @@
       <c r="B7" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
@@ -1603,7 +1627,9 @@
       <c r="B8" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
@@ -1657,7 +1683,9 @@
       <c r="B9" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
@@ -1711,7 +1739,9 @@
       <c r="B10" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
@@ -1765,7 +1795,9 @@
       <c r="B11" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="10"/>
+      <c r="C11" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10" t="s">
@@ -1819,7 +1851,9 @@
       <c r="B12" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="9" t="s">
@@ -1871,7 +1905,9 @@
       <c r="B13" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="10"/>
+      <c r="C13" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10" t="s">
@@ -1927,7 +1963,9 @@
       <c r="B14" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C14" s="10"/>
+      <c r="C14" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
@@ -1985,7 +2023,9 @@
       <c r="B15" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10" t="s">
@@ -2041,7 +2081,9 @@
       <c r="B16" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10" t="s">
@@ -2090,14 +2132,16 @@
       </c>
       <c r="V16" s="9"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
         <v>121</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="10" t="s">
+        <v>201</v>
+      </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10" t="s">
@@ -2153,7 +2197,9 @@
       <c r="B18" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="C18" s="19"/>
+      <c r="C18" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="9"/>
@@ -2191,7 +2237,9 @@
       <c r="B19" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="C19" s="20"/>
+      <c r="C19" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
       <c r="F19" s="9"/>
@@ -2227,7 +2275,9 @@
       <c r="B20" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="C20" s="20"/>
+      <c r="C20" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="9"/>
@@ -2263,7 +2313,9 @@
       <c r="B21" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="C21" s="20"/>
+      <c r="C21" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="9"/>
@@ -2297,37 +2349,37 @@
         <v>121</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="20" t="s">
         <v>36</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="H22" s="20">
         <v>3036</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M22" s="9"/>
       <c r="N22" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="9" t="s">
@@ -2347,16 +2399,18 @@
         <v>121</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="C23" s="20"/>
+        <v>178</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>199</v>
+      </c>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
       <c r="F23" s="20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H23" s="20">
         <v>3034</v>
@@ -2385,13 +2439,15 @@
         <v>121</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="C24" s="20"/>
+        <v>181</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>200</v>
+      </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G24" s="9"/>
       <c r="H24" s="19"/>
@@ -2429,22 +2485,22 @@
       <c r="H25" s="19"/>
       <c r="I25" s="19"/>
       <c r="J25" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="M25" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="N25" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="O25" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="P25" s="12" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Adding directories per each instance
</commit_message>
<xml_diff>
--- a/data/instances.xlsx
+++ b/data/instances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gxologistics-my.sharepoint.com/personal/xavier_parro_gxo_com/Documents/1. GXO/3. Internal/3. Developments/2. BY Instances Manager/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{3A3C676D-04FE-46A3-BA85-E52D00AEE8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13A16423-F262-4F25-9FDB-1632211FCF09}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{3A3C676D-04FE-46A3-BA85-E52D00AEE8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA7964AD-76E1-4156-9A58-74998BFCC424}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="816" windowWidth="23256" windowHeight="13896" xr2:uid="{3AFE9030-45BA-40A4-AA93-EF8467272483}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="201">
   <si>
     <t>GXO  Account</t>
   </si>
@@ -610,9 +610,6 @@
     <t>CONSOLE PROD</t>
   </si>
   <si>
-    <t>WhID</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
@@ -631,15 +628,9 @@
     <t>GE1</t>
   </si>
   <si>
-    <t>Kumho</t>
-  </si>
-  <si>
     <t>Kumo Tires</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
@@ -647,13 +638,16 @@
   </si>
   <si>
     <t>Netherlands</t>
+  </si>
+  <si>
+    <t>US</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -709,6 +703,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -814,7 +823,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -862,6 +871,12 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1197,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A76667-0CAD-4F16-B578-156EFED1F1DC}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1211,12 +1226,11 @@
     <col min="4" max="4" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6328125" customWidth="1"/>
-    <col min="10" max="10" width="54.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="54.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="54.1796875" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="54.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1224,13 +1238,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>192</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>2</v>
@@ -1241,50 +1255,47 @@
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="I1" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="R1" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="S1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="T1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
@@ -1292,7 +1303,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -1305,42 +1316,41 @@
       <c r="H2" s="23">
         <v>1722</v>
       </c>
-      <c r="I2" s="23"/>
+      <c r="I2" s="26" t="s">
+        <v>16</v>
+      </c>
       <c r="J2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>18</v>
       </c>
+      <c r="L2" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="M2" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="O2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="R2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="S2" s="15" t="s">
         <v>25</v>
       </c>
+      <c r="T2" s="9"/>
       <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -1348,7 +1358,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -1361,42 +1371,41 @@
       <c r="H3" s="20">
         <v>3022</v>
       </c>
-      <c r="I3" s="20"/>
+      <c r="I3" s="26" t="s">
+        <v>29</v>
+      </c>
       <c r="J3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>31</v>
       </c>
+      <c r="L3" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="M3" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="O3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="R3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="S3" s="15" t="s">
         <v>25</v>
       </c>
+      <c r="T3" s="9"/>
       <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>12</v>
       </c>
@@ -1404,7 +1413,7 @@
         <v>35</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -1417,42 +1426,41 @@
       <c r="H4" s="20">
         <v>3001</v>
       </c>
-      <c r="I4" s="20"/>
+      <c r="I4" s="26" t="s">
+        <v>38</v>
+      </c>
       <c r="J4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="K4" s="13" t="s">
         <v>40</v>
       </c>
+      <c r="L4" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="M4" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="O4" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="O4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="R4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S4" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="T4" s="15" t="s">
+      <c r="S4" s="15" t="s">
         <v>25</v>
       </c>
+      <c r="T4" s="9"/>
       <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
@@ -1460,7 +1468,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -1473,42 +1481,41 @@
       <c r="H5" s="20">
         <v>3006</v>
       </c>
-      <c r="I5" s="20"/>
+      <c r="I5" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="J5" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="K5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="K5" s="13" t="s">
         <v>50</v>
       </c>
+      <c r="L5" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="M5" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="O5" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="P5" s="14" t="s">
+      <c r="O5" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="R5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="T5" s="15" t="s">
+      <c r="S5" s="15" t="s">
         <v>25</v>
       </c>
+      <c r="T5" s="9"/>
       <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
@@ -1516,7 +1523,7 @@
         <v>54</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -1529,42 +1536,41 @@
       <c r="H6" s="20">
         <v>3008</v>
       </c>
-      <c r="I6" s="20"/>
+      <c r="I6" s="26" t="s">
+        <v>57</v>
+      </c>
       <c r="J6" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="K6" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="K6" s="13" t="s">
         <v>59</v>
       </c>
+      <c r="L6" s="12" t="s">
+        <v>60</v>
+      </c>
       <c r="M6" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="O6" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="O6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="R6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="T6" s="15" t="s">
+      <c r="S6" s="15" t="s">
         <v>25</v>
       </c>
+      <c r="T6" s="9"/>
       <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
@@ -1572,7 +1578,7 @@
         <v>64</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -1585,42 +1591,41 @@
       <c r="H7" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="18"/>
+      <c r="I7" s="26" t="s">
+        <v>68</v>
+      </c>
       <c r="J7" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="K7" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="K7" s="13" t="s">
         <v>70</v>
       </c>
+      <c r="L7" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="M7" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="O7" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="P7" s="14" t="s">
+      <c r="O7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="R7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S7" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="T7" s="15" t="s">
+      <c r="S7" s="15" t="s">
         <v>25</v>
       </c>
+      <c r="T7" s="9"/>
       <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
@@ -1628,7 +1633,7 @@
         <v>75</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -1641,42 +1646,41 @@
       <c r="H8" s="20">
         <v>3014</v>
       </c>
-      <c r="I8" s="20"/>
+      <c r="I8" s="26" t="s">
+        <v>78</v>
+      </c>
       <c r="J8" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="K8" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="K8" s="13" t="s">
         <v>80</v>
       </c>
+      <c r="L8" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="M8" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="O8" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="P8" s="14" t="s">
+      <c r="O8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="R8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S8" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="T8" s="15" t="s">
+      <c r="S8" s="15" t="s">
         <v>25</v>
       </c>
+      <c r="T8" s="9"/>
       <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -1684,7 +1688,7 @@
         <v>84</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -1697,42 +1701,41 @@
       <c r="H9" s="20">
         <v>3009</v>
       </c>
-      <c r="I9" s="20"/>
+      <c r="I9" s="26" t="s">
+        <v>87</v>
+      </c>
       <c r="J9" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="K9" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="K9" s="13" t="s">
         <v>89</v>
       </c>
+      <c r="L9" s="12" t="s">
+        <v>90</v>
+      </c>
       <c r="M9" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="O9" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="P9" s="14" t="s">
+      <c r="O9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="R9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="T9" s="15" t="s">
+      <c r="S9" s="15" t="s">
         <v>25</v>
       </c>
+      <c r="T9" s="9"/>
       <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
@@ -1740,7 +1743,7 @@
         <v>93</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -1753,42 +1756,41 @@
       <c r="H10" s="23">
         <v>3016</v>
       </c>
-      <c r="I10" s="23"/>
+      <c r="I10" s="26" t="s">
+        <v>96</v>
+      </c>
       <c r="J10" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="K10" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="K10" s="13" t="s">
         <v>98</v>
       </c>
+      <c r="L10" s="12" t="s">
+        <v>99</v>
+      </c>
       <c r="M10" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="O10" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="P10" s="14" t="s">
+      <c r="O10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="R10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S10" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="T10" s="15" t="s">
+      <c r="S10" s="15" t="s">
         <v>25</v>
       </c>
+      <c r="T10" s="9"/>
       <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
@@ -1796,7 +1798,7 @@
         <v>103</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -1809,42 +1811,41 @@
       <c r="H11" s="20">
         <v>3023</v>
       </c>
-      <c r="I11" s="20"/>
+      <c r="I11" s="26" t="s">
+        <v>106</v>
+      </c>
       <c r="J11" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="K11" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="K11" s="13" t="s">
         <v>108</v>
       </c>
+      <c r="L11" s="12" t="s">
+        <v>109</v>
+      </c>
       <c r="M11" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="O11" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="O11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="R11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S11" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="T11" s="15" t="s">
+      <c r="S11" s="15" t="s">
         <v>25</v>
       </c>
+      <c r="T11" s="9"/>
       <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
@@ -1852,7 +1853,7 @@
         <v>112</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -1865,40 +1866,39 @@
       <c r="H12" s="20">
         <v>3009</v>
       </c>
-      <c r="I12" s="20"/>
+      <c r="I12" s="26" t="s">
+        <v>115</v>
+      </c>
       <c r="J12" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="K12" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="K12" s="13" t="s">
         <v>117</v>
       </c>
+      <c r="L12" s="12" t="s">
+        <v>118</v>
+      </c>
       <c r="M12" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="O12" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="P12" s="14" t="s">
+      <c r="O12" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9" t="s">
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="S12" s="9"/>
-      <c r="T12" s="15" t="s">
+      <c r="R12" s="9"/>
+      <c r="S12" s="15" t="s">
         <v>25</v>
       </c>
+      <c r="T12" s="9"/>
       <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>121</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>122</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -1919,44 +1919,43 @@
       <c r="H13" s="20">
         <v>3010</v>
       </c>
-      <c r="I13" s="20"/>
+      <c r="I13" s="26" t="s">
+        <v>125</v>
+      </c>
       <c r="J13" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="K13" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="L13" s="13" t="s">
+      <c r="K13" s="13" t="s">
         <v>127</v>
       </c>
+      <c r="L13" s="12" t="s">
+        <v>128</v>
+      </c>
       <c r="M13" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="O13" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="P13" s="14" t="s">
+      <c r="O13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q13" s="10" t="s">
+      <c r="P13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="Q13" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="S13" s="17" t="s">
+      <c r="R13" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9">
+      <c r="S13" s="9"/>
+      <c r="T13" s="9">
         <v>2025.3</v>
       </c>
-      <c r="V13" s="9"/>
+      <c r="U13" s="9"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>121</v>
       </c>
@@ -1964,7 +1963,7 @@
         <v>133</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -1977,46 +1976,45 @@
       <c r="H14" s="23">
         <v>3027</v>
       </c>
-      <c r="I14" s="23"/>
+      <c r="I14" s="26" t="s">
+        <v>136</v>
+      </c>
       <c r="J14" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="K14" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="K14" s="13" t="s">
         <v>138</v>
       </c>
+      <c r="L14" s="12" t="s">
+        <v>139</v>
+      </c>
       <c r="M14" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="O14" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="P14" s="14" t="s">
+      <c r="O14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q14" s="10" t="s">
+      <c r="P14" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="R14" s="9" t="s">
+      <c r="Q14" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="S14" s="17" t="s">
+      <c r="R14" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="T14" s="15" t="s">
+      <c r="S14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="U14" s="9">
+      <c r="T14" s="9">
         <v>2025.3</v>
       </c>
-      <c r="V14" s="9"/>
+      <c r="U14" s="9"/>
     </row>
-    <row r="15" spans="1:22" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>121</v>
       </c>
@@ -2024,7 +2022,7 @@
         <v>143</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -2037,44 +2035,43 @@
       <c r="H15" s="23">
         <v>3028</v>
       </c>
-      <c r="I15" s="23"/>
+      <c r="I15" s="26" t="s">
+        <v>146</v>
+      </c>
       <c r="J15" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="K15" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="K15" s="13" t="s">
         <v>148</v>
       </c>
+      <c r="L15" s="12" t="s">
+        <v>149</v>
+      </c>
       <c r="M15" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="O15" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="P15" s="14" t="s">
+      <c r="O15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q15" s="10" t="s">
+      <c r="P15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="R15" s="9" t="s">
+      <c r="Q15" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="S15" s="17" t="s">
+      <c r="R15" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9">
+      <c r="S15" s="9"/>
+      <c r="T15" s="9">
         <v>2025.3</v>
       </c>
-      <c r="V15" s="9"/>
+      <c r="U15" s="9"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>121</v>
       </c>
@@ -2082,7 +2079,7 @@
         <v>152</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -2095,44 +2092,43 @@
       <c r="H16" s="24">
         <v>3031</v>
       </c>
-      <c r="I16" s="24"/>
+      <c r="I16" s="26" t="s">
+        <v>155</v>
+      </c>
       <c r="J16" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="K16" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="L16" s="13" t="s">
+      <c r="K16" s="13" t="s">
         <v>157</v>
       </c>
+      <c r="L16" s="12" t="s">
+        <v>158</v>
+      </c>
       <c r="M16" s="12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="O16" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="P16" s="14" t="s">
+      <c r="O16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q16" s="10" t="s">
+      <c r="P16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="R16" s="9" t="s">
+      <c r="Q16" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="S16" s="17" t="s">
+      <c r="R16" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="T16" s="9"/>
-      <c r="U16" s="9">
+      <c r="S16" s="9"/>
+      <c r="T16" s="9">
         <v>2025.3</v>
       </c>
-      <c r="V16" s="9"/>
+      <c r="U16" s="9"/>
     </row>
-    <row r="17" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
         <v>121</v>
       </c>
@@ -2140,7 +2136,7 @@
         <v>161</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -2153,44 +2149,43 @@
       <c r="H17" s="20">
         <v>3032</v>
       </c>
-      <c r="I17" s="20"/>
+      <c r="I17" s="26" t="s">
+        <v>163</v>
+      </c>
       <c r="J17" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="K17" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="K17" s="13" t="s">
         <v>165</v>
       </c>
+      <c r="L17" s="12" t="s">
+        <v>166</v>
+      </c>
       <c r="M17" s="12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="O17" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="P17" s="14" t="s">
+      <c r="O17" s="14" t="s">
         <v>22</v>
       </c>
+      <c r="P17" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="Q17" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="R17" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="S17" s="17" t="s">
+      <c r="R17" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9">
+      <c r="S17" s="9"/>
+      <c r="T17" s="9">
         <v>2025.3</v>
       </c>
-      <c r="V17" s="9"/>
+      <c r="U17" s="9"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>121</v>
       </c>
@@ -2198,39 +2193,38 @@
         <v>170</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="9"/>
       <c r="G18" s="19"/>
       <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
+      <c r="I18" s="27"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
+      <c r="O18" s="9" t="s">
+        <v>171</v>
+      </c>
       <c r="P18" s="9" t="s">
-        <v>171</v>
+        <v>6</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="R18" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="S18" s="17" t="s">
+      <c r="R18" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9">
+      <c r="S18" s="9"/>
+      <c r="T18" s="9">
         <v>2025.3</v>
       </c>
-      <c r="V18" s="9"/>
+      <c r="U18" s="9"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
         <v>121</v>
       </c>
@@ -2238,7 +2232,7 @@
         <v>172</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
@@ -2249,26 +2243,25 @@
       <c r="H19" s="21">
         <v>3035</v>
       </c>
-      <c r="I19" s="21"/>
+      <c r="I19" s="27"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
+      <c r="O19" s="9" t="s">
+        <v>171</v>
+      </c>
       <c r="P19" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R19" s="9"/>
-      <c r="S19" s="17"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="9"/>
       <c r="T19" s="9"/>
       <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
         <v>121</v>
       </c>
@@ -2276,7 +2269,7 @@
         <v>174</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
@@ -2287,26 +2280,25 @@
       <c r="H20" s="21">
         <v>3025</v>
       </c>
-      <c r="I20" s="21"/>
+      <c r="I20" s="27"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
+      <c r="O20" s="9" t="s">
+        <v>171</v>
+      </c>
       <c r="P20" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q20" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R20" s="9"/>
-      <c r="S20" s="17"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="9"/>
       <c r="T20" s="9"/>
       <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="s">
         <v>121</v>
       </c>
@@ -2314,7 +2306,7 @@
         <v>175</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -2325,84 +2317,86 @@
       <c r="H21" s="20">
         <v>3026</v>
       </c>
-      <c r="I21" s="20"/>
+      <c r="I21" s="27"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
+      <c r="O21" s="9" t="s">
+        <v>171</v>
+      </c>
       <c r="P21" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q21" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R21" s="9"/>
-      <c r="S21" s="17"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="9"/>
       <c r="T21" s="9"/>
       <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
     </row>
-    <row r="22" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
         <v>121</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C22" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>193</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>194</v>
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="20" t="s">
         <v>36</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H22" s="20">
         <v>3036</v>
       </c>
-      <c r="I22" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="J22" s="12" t="s">
+      <c r="I22" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="K22" s="9"/>
-      <c r="L22" s="22" t="s">
+      <c r="J22" s="9"/>
+      <c r="K22" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="M22" s="9"/>
-      <c r="N22" s="12" t="s">
+      <c r="L22" s="9"/>
+      <c r="M22" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="O22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9" t="s">
+        <v>171</v>
+      </c>
       <c r="P22" s="9" t="s">
-        <v>171</v>
+        <v>6</v>
       </c>
       <c r="Q22" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="R22" s="9"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="9"/>
+        <v>142</v>
+      </c>
+      <c r="R22" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9">
+        <v>2025.3</v>
+      </c>
       <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
         <v>121</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="C23" s="20" t="s">
-        <v>199</v>
+      <c r="C23" s="10" t="s">
+        <v>200</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
@@ -2415,26 +2409,25 @@
       <c r="H23" s="20">
         <v>3034</v>
       </c>
-      <c r="I23" s="20"/>
+      <c r="I23" s="27"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
+      <c r="O23" s="9" t="s">
+        <v>171</v>
+      </c>
       <c r="P23" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q23" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R23" s="9"/>
-      <c r="S23" s="17"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="9"/>
       <c r="T23" s="9"/>
       <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
         <v>121</v>
       </c>
@@ -2442,7 +2435,7 @@
         <v>181</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
@@ -2451,26 +2444,25 @@
       </c>
       <c r="G24" s="9"/>
       <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
+      <c r="I24" s="27"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
+      <c r="O24" s="9" t="s">
+        <v>171</v>
+      </c>
       <c r="P24" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q24" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R24" s="9"/>
-      <c r="S24" s="17"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="9"/>
       <c r="T24" s="9"/>
       <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="16" t="s">
         <v>121</v>
       </c>
@@ -2483,14 +2475,16 @@
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
+      <c r="I25" s="26" t="s">
+        <v>183</v>
+      </c>
       <c r="J25" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="K25" s="12" t="s">
+      <c r="K25" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="L25" s="13" t="s">
+      <c r="L25" s="12" t="s">
         <v>183</v>
       </c>
       <c r="M25" s="12" t="s">
@@ -2500,68 +2494,65 @@
         <v>183</v>
       </c>
       <c r="O25" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="P25" s="12" t="s">
         <v>22</v>
       </c>
+      <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9">
+      <c r="U25" s="9">
         <v>2023.1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{3766F350-F3F2-4933-92CE-7B7E27579E60}"/>
-    <hyperlink ref="K3" r:id="rId2" display="https://be40-gxo-wms-web-pr2.jdadelivers.com/" xr:uid="{63EDC0B2-B082-4318-8576-4C672AE26F70}"/>
-    <hyperlink ref="K4" r:id="rId3" xr:uid="{84B15FD6-E899-4E72-8C6B-D2A13BB79D3E}"/>
-    <hyperlink ref="K5" r:id="rId4" display="https://be40-gxo-wms-web-pr5.jdadelivers.com/" xr:uid="{193BA167-84F1-464F-953F-06275EB7E036}"/>
-    <hyperlink ref="K6" r:id="rId5" display="https://be40-gxo-wms-web-pr6.jdadelivers.com/" xr:uid="{F357A98C-273C-4C1C-BB2C-E615CF19C4FD}"/>
-    <hyperlink ref="K8" r:id="rId6" xr:uid="{BCCF5E37-A0F5-467E-A67E-252DBE4CF182}"/>
-    <hyperlink ref="K7" r:id="rId7" xr:uid="{E7F1F6A8-3769-4AD6-B39E-25CFCC25D0CB}"/>
-    <hyperlink ref="K9" r:id="rId8" xr:uid="{17CE80FA-9171-434F-ACCE-5E7F0DFB5C04}"/>
-    <hyperlink ref="K10" r:id="rId9" xr:uid="{57FA6B8D-B0B6-46F7-AAE8-6CC96D3FB20F}"/>
-    <hyperlink ref="K11" r:id="rId10" xr:uid="{4B932A32-2155-4640-9201-C88F89212E17}"/>
-    <hyperlink ref="K12:K16" r:id="rId11" display="https://be40-gxo-wms-web-pr7.jdadelivers.com/ " xr:uid="{B2FCD20A-AB1F-4A61-B064-0A5C4677412A}"/>
-    <hyperlink ref="K12" r:id="rId12" xr:uid="{C1B57ABF-D275-4B15-9586-2DB52B1EAD96}"/>
-    <hyperlink ref="K13" r:id="rId13" xr:uid="{8A56D612-1327-4430-B793-F29F05BA7D49}"/>
-    <hyperlink ref="K14" r:id="rId14" xr:uid="{D25D6E68-07BF-4E16-8111-337209DD0A9E}"/>
-    <hyperlink ref="K15" r:id="rId15" xr:uid="{45B67D57-48AA-4979-9DD4-95C145EF8902}"/>
-    <hyperlink ref="K16" r:id="rId16" xr:uid="{8D4D2241-B0B3-402D-90B1-AB3667FC7E33}"/>
-    <hyperlink ref="K25" r:id="rId17" xr:uid="{B52587CA-EB88-4288-AA87-814FB3791748}"/>
-    <hyperlink ref="J2" r:id="rId18" xr:uid="{C03ED2FC-463B-42D8-93AA-F64535F5457C}"/>
-    <hyperlink ref="J3" r:id="rId19" xr:uid="{427E1ACF-1681-4AAF-A714-FDE44D8B1B6E}"/>
-    <hyperlink ref="J4" r:id="rId20" display="https://be40-gxo-wms-web-pr3.jdadelivers.com/ " xr:uid="{83641F08-DF10-4601-8EA9-E259B6B5E955}"/>
-    <hyperlink ref="J5" r:id="rId21" display="https://be40-gxo-wms-web-pr5.jdadelivers.com/" xr:uid="{DD7F49C9-96FE-4171-B5F9-33FD1446AA54}"/>
-    <hyperlink ref="J6" r:id="rId22" display="https://be40-gxo-wms-web-pr6.jdadelivers.com/" xr:uid="{A2464084-721C-4686-91A8-A1F84023EA27}"/>
-    <hyperlink ref="J8" r:id="rId23" display="https://be40-gxo-wms-web-pr8.jdadelivers.com" xr:uid="{A3B32520-2C8F-4AD6-8E04-582D3188ED82}"/>
-    <hyperlink ref="J7" r:id="rId24" display="https://be40-gxo-wms-web-pr7.jdadelivers.com/ " xr:uid="{58C5FAE6-D7BC-486E-BD1F-1A6408E653E6}"/>
-    <hyperlink ref="J9" r:id="rId25" display="https://be40-gxo-wms-web-pr10.jdadelivers.com/ " xr:uid="{904C0D8F-4728-4935-89D5-8CA9173B396F}"/>
-    <hyperlink ref="J10" r:id="rId26" display="https://be40-gxo-wms-web-pr11.jdadelivers.com/ " xr:uid="{66011184-BA8C-4E11-A6DB-8B277D44785E}"/>
-    <hyperlink ref="J11" r:id="rId27" display="https://be40-gxo-wms-web-pr12.jdadelivers.com/ " xr:uid="{D0D2B1BE-AE01-45E0-9564-950F43131EC5}"/>
-    <hyperlink ref="J12:J16" r:id="rId28" display="https://be40-gxo-wms-web-pr7.jdadelivers.com/ " xr:uid="{154A2DF3-883B-4E1E-B3A3-E6F23024EC2F}"/>
-    <hyperlink ref="J12" r:id="rId29" display="https://be40-gxo-wms-web-pr13.jdadelivers.com/ " xr:uid="{0032CB17-0BE7-456F-8B31-23F3B477C3F1}"/>
-    <hyperlink ref="J13" r:id="rId30" display="https://be40-gxo-wms-web-pr14.jdadelivers.com/ " xr:uid="{AE01D5AC-D4CF-4A89-8859-F89B45CE7B80}"/>
-    <hyperlink ref="J14" r:id="rId31" display="https://be40-gxo-wms-web-pr15.jdadelivers.com/ " xr:uid="{6C890227-4BCA-4B5C-9FDC-3A073F40D914}"/>
-    <hyperlink ref="J15" r:id="rId32" display="https://be40-gxo-wms-web-pr17.jdadelivers.com/ " xr:uid="{E2C7C142-575B-45B8-A4FC-DE763D87D763}"/>
-    <hyperlink ref="J16" r:id="rId33" display="https://be40-gxo-wms-web-pr18.jdadelivers.com/ " xr:uid="{A22DA444-5F87-4B32-8D70-818A2C5D7F33}"/>
-    <hyperlink ref="J25" r:id="rId34" xr:uid="{3FA5B2CA-67C6-4642-899E-81BE528BD8F4}"/>
-    <hyperlink ref="J22" r:id="rId35" xr:uid="{9EF87C6B-F674-4009-A22A-2F87F0EB0F82}"/>
-    <hyperlink ref="K17" r:id="rId36" xr:uid="{7B874DA4-C4DD-47D8-8E23-BA6D97AE94E8}"/>
-    <hyperlink ref="J17" r:id="rId37" xr:uid="{05EE619A-F2CD-49C0-8F9F-BB7E6423B829}"/>
-    <hyperlink ref="M25" r:id="rId38" xr:uid="{AF5C4ABA-651D-4526-8102-820EEAED4580}"/>
-    <hyperlink ref="L17" r:id="rId39" xr:uid="{500D6F3A-9711-4F3E-A8D4-F89E5164D01B}"/>
-    <hyperlink ref="L13" r:id="rId40" xr:uid="{8E1BBA83-6589-4B41-9548-3DE700807D2C}"/>
-    <hyperlink ref="M17" r:id="rId41" xr:uid="{75E04D4A-8647-4078-B6CA-7E342011F78D}"/>
-    <hyperlink ref="O25" r:id="rId42" xr:uid="{C26F05ED-D976-4E85-A405-4693D0B788CD}"/>
-    <hyperlink ref="N22" r:id="rId43" xr:uid="{1899FBAE-518F-47B3-A40B-733E036E3781}"/>
-    <hyperlink ref="O17" r:id="rId44" xr:uid="{90888C9B-C7A1-46B7-AB89-F5A1E0410820}"/>
-    <hyperlink ref="L2" r:id="rId45" xr:uid="{E7AC33B2-AD4E-47D8-9C63-357C1CAC541A}"/>
-    <hyperlink ref="L4" r:id="rId46" xr:uid="{D08D73AF-5AE3-487A-8EA5-187EE35BA404}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{3766F350-F3F2-4933-92CE-7B7E27579E60}"/>
+    <hyperlink ref="J3" r:id="rId2" display="https://be40-gxo-wms-web-pr2.jdadelivers.com/" xr:uid="{63EDC0B2-B082-4318-8576-4C672AE26F70}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{84B15FD6-E899-4E72-8C6B-D2A13BB79D3E}"/>
+    <hyperlink ref="J5" r:id="rId4" display="https://be40-gxo-wms-web-pr5.jdadelivers.com/" xr:uid="{193BA167-84F1-464F-953F-06275EB7E036}"/>
+    <hyperlink ref="J6" r:id="rId5" display="https://be40-gxo-wms-web-pr6.jdadelivers.com/" xr:uid="{F357A98C-273C-4C1C-BB2C-E615CF19C4FD}"/>
+    <hyperlink ref="J8" r:id="rId6" xr:uid="{BCCF5E37-A0F5-467E-A67E-252DBE4CF182}"/>
+    <hyperlink ref="J7" r:id="rId7" xr:uid="{E7F1F6A8-3769-4AD6-B39E-25CFCC25D0CB}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{17CE80FA-9171-434F-ACCE-5E7F0DFB5C04}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{57FA6B8D-B0B6-46F7-AAE8-6CC96D3FB20F}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{4B932A32-2155-4640-9201-C88F89212E17}"/>
+    <hyperlink ref="J12:J16" r:id="rId11" display="https://be40-gxo-wms-web-pr7.jdadelivers.com/ " xr:uid="{B2FCD20A-AB1F-4A61-B064-0A5C4677412A}"/>
+    <hyperlink ref="J12" r:id="rId12" xr:uid="{C1B57ABF-D275-4B15-9586-2DB52B1EAD96}"/>
+    <hyperlink ref="J13" r:id="rId13" xr:uid="{8A56D612-1327-4430-B793-F29F05BA7D49}"/>
+    <hyperlink ref="J14" r:id="rId14" xr:uid="{D25D6E68-07BF-4E16-8111-337209DD0A9E}"/>
+    <hyperlink ref="J15" r:id="rId15" xr:uid="{45B67D57-48AA-4979-9DD4-95C145EF8902}"/>
+    <hyperlink ref="J16" r:id="rId16" xr:uid="{8D4D2241-B0B3-402D-90B1-AB3667FC7E33}"/>
+    <hyperlink ref="J25" r:id="rId17" xr:uid="{B52587CA-EB88-4288-AA87-814FB3791748}"/>
+    <hyperlink ref="I2" r:id="rId18" xr:uid="{C03ED2FC-463B-42D8-93AA-F64535F5457C}"/>
+    <hyperlink ref="I3" r:id="rId19" xr:uid="{427E1ACF-1681-4AAF-A714-FDE44D8B1B6E}"/>
+    <hyperlink ref="I4" r:id="rId20" display="https://be40-gxo-wms-web-pr3.jdadelivers.com/ " xr:uid="{83641F08-DF10-4601-8EA9-E259B6B5E955}"/>
+    <hyperlink ref="I5" r:id="rId21" display="https://be40-gxo-wms-web-pr5.jdadelivers.com/" xr:uid="{DD7F49C9-96FE-4171-B5F9-33FD1446AA54}"/>
+    <hyperlink ref="I6" r:id="rId22" display="https://be40-gxo-wms-web-pr6.jdadelivers.com/" xr:uid="{A2464084-721C-4686-91A8-A1F84023EA27}"/>
+    <hyperlink ref="I8" r:id="rId23" display="https://be40-gxo-wms-web-pr8.jdadelivers.com" xr:uid="{A3B32520-2C8F-4AD6-8E04-582D3188ED82}"/>
+    <hyperlink ref="I7" r:id="rId24" display="https://be40-gxo-wms-web-pr7.jdadelivers.com/ " xr:uid="{58C5FAE6-D7BC-486E-BD1F-1A6408E653E6}"/>
+    <hyperlink ref="I9" r:id="rId25" display="https://be40-gxo-wms-web-pr10.jdadelivers.com/ " xr:uid="{904C0D8F-4728-4935-89D5-8CA9173B396F}"/>
+    <hyperlink ref="I10" r:id="rId26" display="https://be40-gxo-wms-web-pr11.jdadelivers.com/ " xr:uid="{66011184-BA8C-4E11-A6DB-8B277D44785E}"/>
+    <hyperlink ref="I11" r:id="rId27" display="https://be40-gxo-wms-web-pr12.jdadelivers.com/ " xr:uid="{D0D2B1BE-AE01-45E0-9564-950F43131EC5}"/>
+    <hyperlink ref="I12:I16" r:id="rId28" display="https://be40-gxo-wms-web-pr7.jdadelivers.com/ " xr:uid="{154A2DF3-883B-4E1E-B3A3-E6F23024EC2F}"/>
+    <hyperlink ref="I12" r:id="rId29" display="https://be40-gxo-wms-web-pr13.jdadelivers.com/ " xr:uid="{0032CB17-0BE7-456F-8B31-23F3B477C3F1}"/>
+    <hyperlink ref="I13" r:id="rId30" display="https://be40-gxo-wms-web-pr14.jdadelivers.com/ " xr:uid="{AE01D5AC-D4CF-4A89-8859-F89B45CE7B80}"/>
+    <hyperlink ref="I14" r:id="rId31" display="https://be40-gxo-wms-web-pr15.jdadelivers.com/ " xr:uid="{6C890227-4BCA-4B5C-9FDC-3A073F40D914}"/>
+    <hyperlink ref="I15" r:id="rId32" display="https://be40-gxo-wms-web-pr17.jdadelivers.com/ " xr:uid="{E2C7C142-575B-45B8-A4FC-DE763D87D763}"/>
+    <hyperlink ref="I16" r:id="rId33" display="https://be40-gxo-wms-web-pr18.jdadelivers.com/ " xr:uid="{A22DA444-5F87-4B32-8D70-818A2C5D7F33}"/>
+    <hyperlink ref="I25" r:id="rId34" xr:uid="{3FA5B2CA-67C6-4642-899E-81BE528BD8F4}"/>
+    <hyperlink ref="I22" r:id="rId35" xr:uid="{9EF87C6B-F674-4009-A22A-2F87F0EB0F82}"/>
+    <hyperlink ref="J17" r:id="rId36" xr:uid="{7B874DA4-C4DD-47D8-8E23-BA6D97AE94E8}"/>
+    <hyperlink ref="I17" r:id="rId37" xr:uid="{05EE619A-F2CD-49C0-8F9F-BB7E6423B829}"/>
+    <hyperlink ref="L25" r:id="rId38" xr:uid="{AF5C4ABA-651D-4526-8102-820EEAED4580}"/>
+    <hyperlink ref="K17" r:id="rId39" xr:uid="{500D6F3A-9711-4F3E-A8D4-F89E5164D01B}"/>
+    <hyperlink ref="K13" r:id="rId40" xr:uid="{8E1BBA83-6589-4B41-9548-3DE700807D2C}"/>
+    <hyperlink ref="L17" r:id="rId41" xr:uid="{75E04D4A-8647-4078-B6CA-7E342011F78D}"/>
+    <hyperlink ref="N25" r:id="rId42" xr:uid="{C26F05ED-D976-4E85-A405-4693D0B788CD}"/>
+    <hyperlink ref="M22" r:id="rId43" xr:uid="{1899FBAE-518F-47B3-A40B-733E036E3781}"/>
+    <hyperlink ref="N17" r:id="rId44" xr:uid="{90888C9B-C7A1-46B7-AB89-F5A1E0410820}"/>
+    <hyperlink ref="K2" r:id="rId45" xr:uid="{E7AC33B2-AD4E-47D8-9C63-357C1CAC541A}"/>
+    <hyperlink ref="K4" r:id="rId46" xr:uid="{D08D73AF-5AE3-487A-8EA5-187EE35BA404}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>